<commit_message>
Changes up to 22/11/23
</commit_message>
<xml_diff>
--- a/Greenfield Model copy/OREIA3_2017/data/investment.xlsx
+++ b/Greenfield Model copy/OREIA3_2017/data/investment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/axel/Desktop/Edinburgh MMath Degree Stuff/MMath Diss/Year5-MMath-Diss/Greenfield Model copy/OREIA3_2017/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC798E20-5F78-634B-8790-3810E54123F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2665CA0B-5048-C643-9EAC-CC8A5F94B78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="740" windowWidth="28320" windowHeight="18380" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13720" yWindow="740" windowWidth="15680" windowHeight="11800" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -1396,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="234" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1582,10 +1582,10 @@
         <v>89</v>
       </c>
       <c r="B13" s="8">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="C13" s="14">
-        <v>7000</v>
+        <v>5000</v>
       </c>
       <c r="D13" s="14">
         <v>25</v>
@@ -1595,11 +1595,11 @@
       <c r="A14" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="6">
-        <v>66137</v>
+      <c r="B14" s="8">
+        <v>15000</v>
       </c>
       <c r="C14" s="4">
-        <v>576</v>
+        <v>0</v>
       </c>
       <c r="D14" s="4">
         <v>25</v>
@@ -1610,10 +1610,10 @@
         <v>91</v>
       </c>
       <c r="B15" s="8">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="C15" s="14">
-        <v>7000</v>
+        <v>5000</v>
       </c>
       <c r="D15" s="4">
         <v>25</v>
@@ -1624,10 +1624,10 @@
         <v>92</v>
       </c>
       <c r="B16" s="8">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="C16" s="14">
-        <v>7000</v>
+        <v>5000</v>
       </c>
       <c r="D16" s="4">
         <v>25</v>

</xml_diff>